<commit_message>
After some database tuning
</commit_message>
<xml_diff>
--- a/db_tuning.xlsx
+++ b/db_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>bez tuningu</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>zapytania:</t>
+  </si>
+  <si>
+    <t>po tuningu:</t>
+  </si>
+  <si>
+    <t>śr zapytania</t>
+  </si>
+  <si>
+    <t>śr po tuningu</t>
+  </si>
+  <si>
+    <t>po jdbc.batch</t>
   </si>
 </sst>
 </file>
@@ -193,24 +205,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="45408256"/>
-        <c:axId val="45410560"/>
+        <c:axId val="77087488"/>
+        <c:axId val="77089024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45408256"/>
+        <c:axId val="77087488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45410560"/>
+        <c:crossAx val="77089024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45410560"/>
+        <c:axId val="77089024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -218,7 +230,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45408256"/>
+        <c:crossAx val="77087488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -231,7 +243,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -250,10 +262,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14776618547681539"/>
-          <c:y val="2.8252405949256341E-2"/>
-          <c:w val="0.64550131233595798"/>
-          <c:h val="0.68921660834062404"/>
+          <c:x val="0.14776618547681547"/>
+          <c:y val="2.8252405949256338E-2"/>
+          <c:w val="0.6455013123359582"/>
+          <c:h val="0.68921660834062382"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -368,24 +380,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48360064"/>
-        <c:axId val="48523904"/>
+        <c:axId val="77121792"/>
+        <c:axId val="78585856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48360064"/>
+        <c:axId val="77121792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48523904"/>
+        <c:crossAx val="78585856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48523904"/>
+        <c:axId val="78585856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +405,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48360064"/>
+        <c:crossAx val="77121792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -406,7 +418,128 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>normalnie</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$D$57:$I$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8322</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>tuning</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$D$66:$I$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="78610816"/>
+        <c:axId val="78612352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="78610816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78612352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78612352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78610816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -447,15 +580,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>447676</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -469,6 +602,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -762,16 +925,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I63"/>
+  <dimension ref="A3:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
@@ -891,7 +1054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>475.96382674916703</v>
       </c>
@@ -899,7 +1062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>480.53820278712101</v>
       </c>
@@ -912,8 +1075,11 @@
       <c r="E18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>517.866390471258</v>
       </c>
@@ -926,8 +1092,11 @@
       <c r="E19">
         <v>132972</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>48917</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>396.66798889329601</v>
       </c>
@@ -938,7 +1107,7 @@
         <v>210895</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>366.16623947272001</v>
       </c>
@@ -949,7 +1118,7 @@
         <v>217203</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>370.23324694557499</v>
       </c>
@@ -957,7 +1126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>367.51194413818399</v>
       </c>
@@ -965,7 +1134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>370.23324694557499</v>
       </c>
@@ -973,7 +1142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>343.52456200618298</v>
       </c>
@@ -981,7 +1150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>364.830353885443</v>
       </c>
@@ -989,7 +1158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>366.16623947272001</v>
       </c>
@@ -997,7 +1166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>371.60906726124102</v>
       </c>
@@ -1005,7 +1174,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>370.23324694557499</v>
       </c>
@@ -1013,7 +1182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>347.10170079833301</v>
       </c>
@@ -1021,7 +1190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>366.16623947272001</v>
       </c>
@@ -1029,7 +1198,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>370.23324694557499</v>
       </c>
@@ -1313,6 +1482,9 @@
       <c r="B56">
         <v>23</v>
       </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
@@ -1355,6 +1527,9 @@
       <c r="B59">
         <v>26</v>
       </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
@@ -1363,6 +1538,24 @@
       <c r="B60">
         <v>27</v>
       </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>4</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>6</v>
+      </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
@@ -1371,6 +1564,24 @@
       <c r="B61">
         <v>28</v>
       </c>
+      <c r="D61">
+        <v>280</v>
+      </c>
+      <c r="E61">
+        <v>310</v>
+      </c>
+      <c r="F61">
+        <v>490</v>
+      </c>
+      <c r="G61">
+        <v>480</v>
+      </c>
+      <c r="H61">
+        <v>690</v>
+      </c>
+      <c r="I61">
+        <v>610</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
@@ -1379,6 +1590,24 @@
       <c r="B62">
         <v>29</v>
       </c>
+      <c r="D62">
+        <v>210</v>
+      </c>
+      <c r="E62">
+        <v>300</v>
+      </c>
+      <c r="F62">
+        <v>330</v>
+      </c>
+      <c r="G62">
+        <v>550</v>
+      </c>
+      <c r="H62">
+        <v>680</v>
+      </c>
+      <c r="I62">
+        <v>700</v>
+      </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
@@ -1386,6 +1615,69 @@
       </c>
       <c r="B63">
         <v>30</v>
+      </c>
+      <c r="D63">
+        <v>250</v>
+      </c>
+      <c r="E63">
+        <v>230</v>
+      </c>
+      <c r="F63">
+        <v>260</v>
+      </c>
+      <c r="G63">
+        <v>420</v>
+      </c>
+      <c r="H63">
+        <v>680</v>
+      </c>
+      <c r="I63">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="D64">
+        <v>250</v>
+      </c>
+      <c r="E64">
+        <v>230</v>
+      </c>
+      <c r="F64">
+        <v>310</v>
+      </c>
+      <c r="G64">
+        <v>680</v>
+      </c>
+      <c r="H64">
+        <v>520</v>
+      </c>
+      <c r="I64">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9">
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9">
+      <c r="D66">
+        <v>247</v>
+      </c>
+      <c r="E66">
+        <v>267</v>
+      </c>
+      <c r="F66">
+        <v>347</v>
+      </c>
+      <c r="G66">
+        <v>532</v>
+      </c>
+      <c r="H66">
+        <v>642</v>
+      </c>
+      <c r="I66">
+        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>